<commit_message>
update Dockerfile and test data
</commit_message>
<xml_diff>
--- a/Local/Data/medData/dqTestData.xlsx
+++ b/Local/Data/medData/dqTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="93">
   <si>
     <t xml:space="preserve">Institut_ID</t>
   </si>
@@ -82,10 +82,10 @@
     <t xml:space="preserve">E75.0</t>
   </si>
   <si>
-    <t xml:space="preserve">Stationär</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erledigt</t>
+    <t xml:space="preserve">IMP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finished</t>
   </si>
   <si>
     <t xml:space="preserve">HD</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">F_101642</t>
   </si>
   <si>
-    <t xml:space="preserve">Ambulant</t>
+    <t xml:space="preserve">AMB</t>
   </si>
   <si>
     <t xml:space="preserve">ND</t>
@@ -314,6 +314,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -399,13 +400,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.71"/>
@@ -413,7 +414,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.73"/>
@@ -685,6 +686,24 @@
       <c r="I6" s="0" t="n">
         <v>586</v>
       </c>
+      <c r="J6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>43561</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>4503</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
@@ -714,6 +733,18 @@
       <c r="I7" s="0" t="n">
         <v>589</v>
       </c>
+      <c r="J7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>43562</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -743,6 +774,18 @@
       <c r="I8" s="0" t="n">
         <v>589</v>
       </c>
+      <c r="J8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>43563</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
@@ -772,6 +815,18 @@
       <c r="I9" s="0" t="n">
         <v>586</v>
       </c>
+      <c r="J9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <v>43564</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -801,6 +856,24 @@
       <c r="I10" s="0" t="n">
         <v>324</v>
       </c>
+      <c r="J10" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <v>43565</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="0" t="n">
+        <v>5303</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
@@ -830,6 +903,24 @@
       <c r="I11" s="0" t="n">
         <v>589</v>
       </c>
+      <c r="J11" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <v>43566</v>
+      </c>
+      <c r="N11" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="0" t="n">
+        <v>5503</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
@@ -856,6 +947,24 @@
       <c r="I12" s="0" t="n">
         <v>586</v>
       </c>
+      <c r="J12" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L12" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <v>43567</v>
+      </c>
+      <c r="N12" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="0" t="n">
+        <v>5703</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
@@ -882,6 +991,24 @@
       <c r="I13" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="J13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <v>43568</v>
+      </c>
+      <c r="N13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="0" t="n">
+        <v>5903</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
@@ -908,6 +1035,24 @@
       <c r="H14" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="J14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <v>43569</v>
+      </c>
+      <c r="N14" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <v>6103</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
@@ -934,6 +1079,24 @@
       <c r="H15" s="0" t="s">
         <v>59</v>
       </c>
+      <c r="J15" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <v>43570</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <v>6303</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
@@ -957,6 +1120,24 @@
       <c r="G16" s="1" t="n">
         <v>43941</v>
       </c>
+      <c r="J16" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <v>43571</v>
+      </c>
+      <c r="N16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <v>6503</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
@@ -986,6 +1167,24 @@
       <c r="I17" s="0" t="n">
         <v>320</v>
       </c>
+      <c r="J17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <v>43572</v>
+      </c>
+      <c r="N17" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O17" s="0" t="n">
+        <v>6703</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
@@ -1015,6 +1214,24 @@
       <c r="I18" s="0" t="n">
         <v>71529</v>
       </c>
+      <c r="J18" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="1" t="n">
+        <v>43573</v>
+      </c>
+      <c r="N18" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>6903</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
@@ -1041,6 +1258,24 @@
       <c r="H19" s="0" t="s">
         <v>64</v>
       </c>
+      <c r="J19" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="1" t="n">
+        <v>43574</v>
+      </c>
+      <c r="N19" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>7103</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
@@ -1067,6 +1302,24 @@
       <c r="H20" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="J20" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="1" t="n">
+        <v>43575</v>
+      </c>
+      <c r="N20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>7303</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
@@ -1093,6 +1346,24 @@
       <c r="H21" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="J21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <v>43576</v>
+      </c>
+      <c r="N21" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="0" t="n">
+        <v>7503</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
@@ -1119,6 +1390,24 @@
       <c r="H22" s="0" t="s">
         <v>76</v>
       </c>
+      <c r="J22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <v>43577</v>
+      </c>
+      <c r="N22" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>7703</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
@@ -1148,6 +1437,24 @@
       <c r="I23" s="0" t="n">
         <v>342</v>
       </c>
+      <c r="J23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="1" t="n">
+        <v>43578</v>
+      </c>
+      <c r="N23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>7903</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -1177,6 +1484,24 @@
       <c r="I24" s="0" t="n">
         <v>226</v>
       </c>
+      <c r="J24" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <v>43579</v>
+      </c>
+      <c r="N24" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="0" t="n">
+        <v>8103</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
@@ -1206,6 +1531,24 @@
       <c r="I25" s="0" t="n">
         <v>324</v>
       </c>
+      <c r="J25" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <v>43580</v>
+      </c>
+      <c r="N25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O25" s="0" t="n">
+        <v>8303</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -1235,6 +1578,24 @@
       <c r="I26" s="0" t="n">
         <v>796</v>
       </c>
+      <c r="J26" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M26" s="1" t="n">
+        <v>43581</v>
+      </c>
+      <c r="N26" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O26" s="0" t="n">
+        <v>8503</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
@@ -1261,6 +1622,24 @@
       <c r="H27" s="0" t="s">
         <v>86</v>
       </c>
+      <c r="J27" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M27" s="1" t="n">
+        <v>43582</v>
+      </c>
+      <c r="N27" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27" s="0" t="n">
+        <v>8703</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -1287,6 +1666,24 @@
       <c r="H28" s="0" t="s">
         <v>89</v>
       </c>
+      <c r="J28" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M28" s="1" t="n">
+        <v>43583</v>
+      </c>
+      <c r="N28" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O28" s="0" t="n">
+        <v>8903</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -1316,6 +1713,24 @@
       <c r="I29" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="J29" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L29" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M29" s="1" t="n">
+        <v>43584</v>
+      </c>
+      <c r="N29" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O29" s="0" t="n">
+        <v>9103</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
@@ -1341,6 +1756,118 @@
       </c>
       <c r="H30" s="0" t="s">
         <v>44</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M30" s="1" t="n">
+        <v>43585</v>
+      </c>
+      <c r="N30" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O30" s="0" t="n">
+        <v>9303</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="1" t="n">
+        <v>55155</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <v>43923</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>796</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M31" s="1" t="n">
+        <v>43581</v>
+      </c>
+      <c r="N31" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O31" s="0" t="n">
+        <v>8503</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>1990</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="1" t="n">
+        <v>55155</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <v>43923</v>
+      </c>
+      <c r="H32" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>796</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="M32" s="1" t="n">
+        <v>43581</v>
+      </c>
+      <c r="N32" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="O32" s="0" t="n">
+        <v>8503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>